<commit_message>
updated structurer for overview
</commit_message>
<xml_diff>
--- a/config/customstopwords.xlsx
+++ b/config/customstopwords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Repos/github.com/DominikFin/nlp-satisfaction/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592857E1-20D2-A64D-A7E7-97D62CB9DA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C94ED8-3D0E-B248-8811-B0D58C9AE761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="1280" windowWidth="12740" windowHeight="13760" xr2:uid="{2C3D0758-7DDE-6C4C-B20E-A7C9901B7270}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="444">
   <si>
     <t>stopword</t>
   </si>
@@ -1368,6 +1368,9 @@
   </si>
   <si>
     <t>offensichtlich</t>
+  </si>
+  <si>
+    <t>bitte</t>
   </si>
 </sst>
 </file>
@@ -1735,10 +1738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E221091-9428-0242-81DB-E4DAAE5CF232}">
-  <dimension ref="A1:A453"/>
+  <dimension ref="A1:A455"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A435" workbookViewId="0">
-      <selection activeCell="A453" sqref="A453"/>
+      <selection activeCell="A457" sqref="A457"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4011,6 +4014,16 @@
         <v>442</v>
       </c>
     </row>
+    <row r="454" spans="1:1" ht="17" x14ac:dyDescent="0.25">
+      <c r="A454" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" ht="17" x14ac:dyDescent="0.25">
+      <c r="A455" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A416" xr:uid="{5E221091-9428-0242-81DB-E4DAAE5CF232}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A416">

</xml_diff>